<commit_message>
User Management & Payroll Fix
</commit_message>
<xml_diff>
--- a/public/excel_files/masterlist-2014-09-08.xlsx
+++ b/public/excel_files/masterlist-2014-09-08.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Payroll Period</t>
   </si>
   <si>
-    <t>2014-09-08-2014-09-08</t>
+    <t>2014-08-01-2014-08-15</t>
   </si>
   <si>
     <t>Payroll Mode</t>
@@ -32,7 +32,7 @@
     <t>Payroll Date</t>
   </si>
   <si>
-    <t>Monthly</t>
+    <t>Semi-monthly</t>
   </si>
   <si>
     <t>Position</t>
@@ -84,6 +84,21 @@
   </si>
   <si>
     <t>Net</t>
+  </si>
+  <si>
+    <t>Web Developer1</t>
+  </si>
+  <si>
+    <t>Jen Dee  Dela Cruz</t>
+  </si>
+  <si>
+    <t>12,500.00</t>
+  </si>
+  <si>
+    <t>1,153.85</t>
+  </si>
+  <si>
+    <t>S0</t>
   </si>
 </sst>
 </file>
@@ -449,7 +464,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="E4" sqref="E4"/>
@@ -553,6 +568,59 @@
         <v>22</v>
       </c>
     </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5">
+        <v>290.65</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
+        <v>12692.30769230769</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>-532.96</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>